<commit_message>
updated mult compare for diel period np
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/diel-period/np/glmm_multi_comp_diel_period_np.xlsx
+++ b/results/accel-glmm-results/diel-period/np/glmm_multi_comp_diel_period_np.xlsx
@@ -1,73 +1,93 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\CU\Data\toronto-lmb-np-accel\results\accel-glmm-results\diel-period\np\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C078855-8013-45E4-95C1-8C2E9CE4A6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t xml:space="preserve">term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contrast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">std_error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">statistic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adj_p_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">day_night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day / Night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dusk / Night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dawn / Night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day / Dusk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dawn / Dusk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dawn / Day</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>contrast</t>
+  </si>
+  <si>
+    <t>null_value</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>std_error</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>statistic</t>
+  </si>
+  <si>
+    <t>adj_p_value</t>
+  </si>
+  <si>
+    <t>day_night</t>
+  </si>
+  <si>
+    <t>Day / Night</t>
+  </si>
+  <si>
+    <t>Dusk / Night</t>
+  </si>
+  <si>
+    <t>Dawn / Night</t>
+  </si>
+  <si>
+    <t>Day / Dusk</t>
+  </si>
+  <si>
+    <t>Dawn / Dusk</t>
+  </si>
+  <si>
+    <t>Dawn / Day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -103,6 +123,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -384,14 +413,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:I13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,182 +451,182 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>1.10654180076353</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.00357818240501286</v>
+      <c r="D2">
+        <v>1.1065418007635299</v>
+      </c>
+      <c r="E2">
+        <v>3.5781824050128601E-3</v>
       </c>
       <c r="F2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
-        <v>31.308049722449</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2.17558249907143e-214</v>
+      <c r="H2">
+        <v>31.308049722448999</v>
+      </c>
+      <c r="I2">
+        <v>2.1755824990714299E-214</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" t="n">
-        <v>1.22740620187603</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.00861457140037816</v>
+      <c r="D3">
+        <v>1.2274062018760299</v>
+      </c>
+      <c r="E3">
+        <v>8.6145714003781591E-3</v>
       </c>
       <c r="F3" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" t="n">
-        <v>29.1946519871464</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000136041215738227</v>
+      <c r="H3">
+        <v>29.194651987146401</v>
+      </c>
+      <c r="I3">
+        <v>1.3604121573822699E-186</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>1.13648854182739</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.00823735244700242</v>
+      <c r="E4">
+        <v>8.2373524470024193E-3</v>
       </c>
       <c r="F4" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" t="n">
-        <v>17.6520399300342</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000588877140096181</v>
+      <c r="H4">
+        <v>17.652039930034199</v>
+      </c>
+      <c r="I4">
+        <v>5.88877140096181E-69</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>0.90152860485163</v>
       </c>
-      <c r="E5" t="n">
-        <v>0.00633368963735631</v>
+      <c r="E5">
+        <v>6.3336896373563101E-3</v>
       </c>
       <c r="F5" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>-14.7553198517334</v>
       </c>
-      <c r="I5" t="n">
-        <v>0.00000000000000000000000000000000000000000000000170604094235732</v>
+      <c r="I5">
+        <v>1.70604094235732E-48</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
-        <v>0.925926999627608</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.00885432137283516</v>
+      <c r="D6">
+        <v>0.92592699962760805</v>
+      </c>
+      <c r="E6">
+        <v>8.8543213728351604E-3</v>
       </c>
       <c r="F6" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>-8.04796090005377</v>
       </c>
-      <c r="I6" t="n">
-        <v>0.00000000000000505108994954994</v>
+      <c r="I6">
+        <v>5.0510899495499397E-15</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" t="n">
-        <v>1.02706336176653</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.00745688308973903</v>
+      <c r="D7">
+        <v>1.0270633617665299</v>
+      </c>
+      <c r="E7">
+        <v>7.4568830897390297E-3</v>
       </c>
       <c r="F7" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>3.67798643921327</v>
       </c>
-      <c r="I7" t="n">
-        <v>0.00141049472932646</v>
+      <c r="I7">
+        <v>1.4104947293264601E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>